<commit_message>
nouveaux tableaux et MAJ graphiques
</commit_message>
<xml_diff>
--- a/scores des modèles.xlsx
+++ b/scores des modèles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Data Science\Desktop\OpenClassrooms\Projets\03 - Anticipez les besoins en consommation de bâtiments\Projet 03 - Fichiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4E449-6443-4D0C-820D-7BE20D55B21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCE7FAF-987F-4B18-9EF2-658E8822BC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>DummyRegressor</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Graphiques</t>
+  </si>
+  <si>
+    <t>R² moyens sur test</t>
+  </si>
+  <si>
+    <t>Durée fit moyen</t>
   </si>
 </sst>
 </file>
@@ -974,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1193,6 +1199,53 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1205,52 +1258,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1318,7 +1354,7 @@
                 </a:solidFill>
                 <a:latin typeface="DIN Alternate" pitchFamily="50" charset="0"/>
               </a:rPr>
-              <a:t>Scores R² moyens - </a:t>
+              <a:t>Scores R² moyens (GridSearchCV) - </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="3200" b="1" baseline="0">
@@ -1354,7 +1390,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22286874970000353"/>
+          <c:x val="0.15070996511758719"/>
           <c:y val="4.3579776305359356E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1868,7 +1904,25 @@
                 </a:solidFill>
                 <a:latin typeface="DIN Alternate" pitchFamily="50" charset="0"/>
               </a:rPr>
-              <a:t>Scores R² moyens - </a:t>
+              <a:t>Scores R² moyens </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:latin typeface="DIN Alternate" pitchFamily="50" charset="0"/>
+              </a:rPr>
+              <a:t>(GridSearchCV) </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="3200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:latin typeface="DIN Alternate" pitchFamily="50" charset="0"/>
+              </a:rPr>
+              <a:t>- </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" sz="3200" b="1" baseline="0">
@@ -3816,7 +3870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW312"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3837,27 +3893,37 @@
     <col min="15" max="15" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" s="11" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="74" t="s">
+    <row r="1" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" s="11" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="77"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="94"/>
     </row>
-    <row r="3" spans="2:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:17" s="11" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="78" t="s">
+    <row r="3" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S3" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="100"/>
+    </row>
+    <row r="4" spans="2:22" s="11" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="79"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
@@ -3880,10 +3946,10 @@
         <v>7</v>
       </c>
       <c r="K4" s="42"/>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="79"/>
+      <c r="M4" s="90"/>
       <c r="N4" s="6" t="s">
         <v>8</v>
       </c>
@@ -3896,8 +3962,20 @@
       <c r="Q4" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="S4" s="95" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="96" t="s">
+        <v>9</v>
+      </c>
+      <c r="U4" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="97" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="2:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="35" t="s">
         <v>12</v>
       </c>
@@ -3944,8 +4022,24 @@
       <c r="Q5" s="1">
         <v>0.63900000000000001</v>
       </c>
+      <c r="S5" s="101">
+        <f>(N6+N12+N22+N28)/4</f>
+        <v>0.65049999999999997</v>
+      </c>
+      <c r="T5" s="101">
+        <f>(O6+O12+O22+O28)/4</f>
+        <v>0.68225000000000002</v>
+      </c>
+      <c r="U5" s="102">
+        <f>(P6+P12+P22+P28)/4</f>
+        <v>0.69074999999999998</v>
+      </c>
+      <c r="V5" s="101">
+        <f>(Q6+Q12+Q22+Q28)/4</f>
+        <v>0.79099999999999993</v>
+      </c>
     </row>
-    <row r="6" spans="2:17" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="55" t="s">
         <v>1</v>
       </c>
@@ -3991,7 +4085,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="53"/>
       <c r="C7" s="52"/>
       <c r="D7" s="50"/>
@@ -4018,8 +4112,14 @@
       <c r="Q7" s="2">
         <v>4191000</v>
       </c>
+      <c r="S7" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" s="103"/>
+      <c r="U7" s="103"/>
+      <c r="V7" s="104"/>
     </row>
-    <row r="8" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="53"/>
       <c r="C8" s="52"/>
       <c r="D8" s="50"/>
@@ -4046,8 +4146,20 @@
       <c r="Q8" s="3">
         <v>2443000</v>
       </c>
+      <c r="S8" s="95" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="96" t="s">
+        <v>9</v>
+      </c>
+      <c r="U8" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="97" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="9" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="53"/>
       <c r="C9" s="52"/>
       <c r="D9" s="51"/>
@@ -4074,8 +4186,24 @@
       <c r="Q9" s="32">
         <v>5640</v>
       </c>
+      <c r="S9" s="101">
+        <f>(N9+N15+N25+N31)/4</f>
+        <v>1545</v>
+      </c>
+      <c r="T9" s="101">
+        <f t="shared" ref="T9:V9" si="0">(O9+O15+O25+O31)/4</f>
+        <v>454</v>
+      </c>
+      <c r="U9" s="101">
+        <f t="shared" si="0"/>
+        <v>201</v>
+      </c>
+      <c r="V9" s="101">
+        <f t="shared" si="0"/>
+        <v>8097.5</v>
+      </c>
     </row>
-    <row r="10" spans="2:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="53"/>
       <c r="C10" s="52"/>
       <c r="D10" s="51"/>
@@ -4103,7 +4231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:17" s="11" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" s="11" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" s="53"/>
       <c r="C11" s="54"/>
       <c r="D11" s="47"/>
@@ -4133,7 +4261,7 @@
         <v>0.61599999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="53"/>
       <c r="C12" s="52"/>
       <c r="D12" s="49"/>
@@ -4161,7 +4289,7 @@
         <v>0.77400000000000002</v>
       </c>
     </row>
-    <row r="13" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="53"/>
       <c r="C13" s="52"/>
       <c r="D13" s="50"/>
@@ -4189,7 +4317,7 @@
         <v>139.69999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="53"/>
       <c r="C14" s="52"/>
       <c r="D14" s="50"/>
@@ -4217,7 +4345,7 @@
         <v>56.81</v>
       </c>
     </row>
-    <row r="15" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="53"/>
       <c r="C15" s="52"/>
       <c r="D15" s="51"/>
@@ -4245,7 +4373,7 @@
         <v>5650</v>
       </c>
     </row>
-    <row r="16" spans="2:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="53"/>
       <c r="C16" s="52"/>
       <c r="D16" s="51"/>
@@ -4275,23 +4403,23 @@
     </row>
     <row r="17" spans="2:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:17" s="11" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="74" t="s">
+      <c r="F18" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="77"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="93"/>
+      <c r="M18" s="94"/>
     </row>
     <row r="19" spans="2:17" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:17" s="11" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="78" t="s">
+      <c r="B20" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="79"/>
+      <c r="C20" s="90"/>
       <c r="D20" s="58" t="s">
         <v>0</v>
       </c>
@@ -4314,10 +4442,10 @@
         <v>7</v>
       </c>
       <c r="K20" s="42"/>
-      <c r="L20" s="78" t="s">
+      <c r="L20" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="M20" s="79"/>
+      <c r="M20" s="90"/>
       <c r="N20" s="6" t="s">
         <v>8</v>
       </c>
@@ -4709,21 +4837,21 @@
     </row>
     <row r="33" spans="1:49" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:49" s="11" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="74" t="s">
+      <c r="F34" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="77"/>
+      <c r="G34" s="92"/>
+      <c r="H34" s="92"/>
+      <c r="I34" s="92"/>
+      <c r="J34" s="92"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="94"/>
     </row>
     <row r="35" spans="1:49" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
-      <c r="C36" s="89"/>
+      <c r="C36" s="74"/>
       <c r="D36" s="6" t="s">
         <v>0</v>
       </c>
@@ -4795,10 +4923,10 @@
     </row>
     <row r="37" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
-      <c r="B37" s="91" t="s">
+      <c r="B37" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="93" t="s">
+      <c r="C37" s="76" t="s">
         <v>25</v>
       </c>
       <c r="D37" s="66">
@@ -4872,8 +5000,8 @@
     </row>
     <row r="38" spans="1:49" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
-      <c r="B38" s="92"/>
-      <c r="C38" s="94" t="s">
+      <c r="B38" s="79"/>
+      <c r="C38" s="77" t="s">
         <v>26</v>
       </c>
       <c r="D38" s="57">
@@ -4947,8 +5075,8 @@
     </row>
     <row r="39" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
-      <c r="B39" s="90"/>
-      <c r="C39" s="90"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
       <c r="O39" s="11"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
@@ -4987,7 +5115,7 @@
     </row>
     <row r="40" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
-      <c r="C40" s="89"/>
+      <c r="C40" s="74"/>
       <c r="D40" s="58" t="s">
         <v>0</v>
       </c>
@@ -5059,10 +5187,10 @@
     </row>
     <row r="41" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="93" t="s">
+      <c r="C41" s="76" t="s">
         <v>25</v>
       </c>
       <c r="D41" s="59">
@@ -5136,8 +5264,8 @@
     </row>
     <row r="42" spans="1:49" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="94" t="s">
+      <c r="B42" s="79"/>
+      <c r="C42" s="77" t="s">
         <v>26</v>
       </c>
       <c r="D42" s="57">
@@ -5480,13 +5608,9 @@
     <row r="311" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="312" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="L21:L26"/>
-    <mergeCell ref="L27:L32"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F34:M34"/>
+  <mergeCells count="15">
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="S7:V7"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="F18:M18"/>
     <mergeCell ref="L4:M4"/>
@@ -5494,9 +5618,15 @@
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="L5:L10"/>
     <mergeCell ref="L11:L16"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="L21:L26"/>
+    <mergeCell ref="L27:L32"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F34:M34"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:J6 N11:Q11">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5508,38 +5638,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:J6">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22:J22 N27:Q27">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -5550,8 +5648,6 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22:J22">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -5573,7 +5669,267 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D22:J22 N27:Q27">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:J22">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D5:K5 N5:Q5">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:K11 N11:Q11">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:K11">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:K21 N21:Q21">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:K21">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:K27 N27:Q27">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:K27">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:N37">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:N38">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:N41">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42:N42">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:Q5">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:Q6">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:Q7">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:Q8">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9:Q9">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10:Q10">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11:Q11">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12:Q12">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -5585,114 +5941,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:K11 N11:Q11">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:K11">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:K21 N21:Q21">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:K21">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:K27 N27:Q27">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:K27">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N5:Q5">
-    <cfRule type="colorScale" priority="68">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N6:Q6">
-    <cfRule type="colorScale" priority="67">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N7:Q7">
-    <cfRule type="colorScale" priority="65">
+  <conditionalFormatting sqref="N13:Q13">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5703,8 +5953,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:Q8">
-    <cfRule type="colorScale" priority="64">
+  <conditionalFormatting sqref="N14:Q14">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5715,8 +5965,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:Q9">
-    <cfRule type="colorScale" priority="63">
+  <conditionalFormatting sqref="N15:Q15">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5727,43 +5977,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10:Q10">
-    <cfRule type="colorScale" priority="62">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N11:Q11">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N12:Q12">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N13:Q13">
+  <conditionalFormatting sqref="N16:Q16">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -5775,44 +5989,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N14:Q14">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15:Q15">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N16:Q16">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N21:Q21">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5824,7 +6002,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:Q22">
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5836,6 +6014,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23:Q23">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N24:Q24">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N25:Q25">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26:Q26">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -5847,31 +6061,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N24:Q24">
+  <conditionalFormatting sqref="N27:Q27">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N25:Q25">
+  <conditionalFormatting sqref="N28:Q28">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26:Q26">
+  <conditionalFormatting sqref="N29:Q29">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -5883,31 +6097,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N27:Q27">
+  <conditionalFormatting sqref="N30:Q30">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28:Q28">
+  <conditionalFormatting sqref="N31:Q31">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N29:Q29">
+  <conditionalFormatting sqref="N32:Q32">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -5919,55 +6133,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30:Q30">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N31:Q31">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N32:Q32">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37:N37">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38:N38">
+  <conditionalFormatting sqref="S5:V5">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -5979,27 +6145,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:N41">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42:N42">
+  <conditionalFormatting sqref="S9:V9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>